<commit_message>
updating the files and cleanup
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_POM\Selenium_POM\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="4305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login_Test_Case_01" sheetId="1" r:id="rId1"/>
-    <sheet name="login_Test_Case_02" sheetId="2" r:id="rId2"/>
+    <sheet name="Google_Search_Test" sheetId="3" r:id="rId2"/>
+    <sheet name="login_Test_Case_02" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -33,6 +38,12 @@
   </si>
   <si>
     <t>May@2017</t>
+  </si>
+  <si>
+    <t>TextToSearch</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
   </si>
 </sst>
 </file>
@@ -365,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +434,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated for multiple rows and parllal execution and tearDown
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="login_Test_Case_01" sheetId="1" r:id="rId1"/>
     <sheet name="Google_Search_Test" sheetId="3" r:id="rId2"/>
-    <sheet name="login_Test_Case_02" sheetId="2" r:id="rId3"/>
+    <sheet name="Google_Search_Test_2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -88,11 +88,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -377,7 +378,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,39 +435,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updating the new files
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login_Test_Case_01" sheetId="1" r:id="rId1"/>
     <sheet name="Google_Search_Test" sheetId="3" r:id="rId2"/>
     <sheet name="Google_Search_Test_2" sheetId="2" r:id="rId3"/>
+    <sheet name="Gmail_Test_1" sheetId="4" r:id="rId4"/>
+    <sheet name="Gmail_Test_2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -44,6 +46,15 @@
   </si>
   <si>
     <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>venkatatest1729@gmail.com</t>
+  </si>
+  <si>
+    <t>Infy@123</t>
   </si>
 </sst>
 </file>
@@ -88,12 +99,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -471,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,4 +505,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>